<commit_message>
metrics: median + deviation
</commit_message>
<xml_diff>
--- a/generated-tests/firebrigade/backend/direct/metrics.xlsx
+++ b/generated-tests/firebrigade/backend/direct/metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marius\Desktop\Bachelor-Arbeit\test-generation-app\generated-tests\firebrigade\backend\direct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262A6124-77C3-41EC-9A07-057EA66ECB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D8E18D6-93AA-469B-986C-2CC9AB0905D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73C55193-3CB0-42EF-A4B9-F7B9A2E05BE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Test</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>createOne, refreshTermsOfRights, findOne, findAll</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Std.-Abw.</t>
+  </si>
+  <si>
+    <t>Standardabweichung</t>
   </si>
 </sst>
 </file>
@@ -823,13 +832,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE60AEF-AC79-4BE5-B0FB-2A2449C95BDE}">
   <dimension ref="C3:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="60.140625" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" customWidth="1"/>
     <col min="6" max="15" width="15.7109375" customWidth="1"/>
@@ -1502,42 +1511,61 @@
       <c r="P25" s="31"/>
     </row>
     <row r="26" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C26" s="32"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
+      <c r="C26" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="26"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31">
+        <f>MEDIAN(K7:K21)</f>
+        <v>5.5</v>
+      </c>
+      <c r="L26" s="31">
+        <f>MEDIAN(L7:L21)</f>
+        <v>8</v>
+      </c>
+      <c r="M26" s="31"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
     </row>
     <row r="27" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C27" s="32"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
+      <c r="C27" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="29">
+        <f>ROUND(_xlfn.STDEV.P(F8,F10,F12,F14,F16,F18,F20,F22),1)</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G27" s="29">
+        <f>ROUND(_xlfn.STDEV.P(G8,G10,G12,G14,G16,G18,G20,G22),1)</f>
+        <v>41.5</v>
+      </c>
+      <c r="H27" s="30">
+        <f>ROUND(_xlfn.STDEV.P(H8,H10,H12,H14,H16,H18,H20,H22),1)</f>
+        <v>18.5</v>
+      </c>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31">
+        <f>ROUND(_xlfn.STDEV.P(K7:K21),1)</f>
+        <v>3.7</v>
+      </c>
+      <c r="L27" s="31">
+        <f>ROUND(_xlfn.STDEV.P(L7:L21),1)</f>
+        <v>5.3</v>
+      </c>
+      <c r="M27" s="31"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
     </row>
     <row r="28" spans="3:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C28" s="32"/>
@@ -1559,9 +1587,15 @@
       <c r="C29" s="32"/>
       <c r="D29" s="10"/>
       <c r="E29" s="14"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="20"/>
+      <c r="F29" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -1575,9 +1609,15 @@
       <c r="C30" s="32"/>
       <c r="D30" s="10"/>
       <c r="E30" s="14"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="20"/>
+      <c r="F30" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="36" t="s">
+        <v>24</v>
+      </c>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>

</xml_diff>